<commit_message>
Commit on 21 feb 2020
</commit_message>
<xml_diff>
--- a/Naukri Login.xlsx
+++ b/Naukri Login.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="6">
   <si>
     <t>Username</t>
   </si>
@@ -371,7 +371,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C231"/>
+  <dimension ref="A1:C232"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -2231,6 +2231,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="232">
+      <c r="A232" t="s">
+        <v>4</v>
+      </c>
+      <c r="B232" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A2"/>

</xml_diff>

<commit_message>
changes for assertion of title in afterclass
</commit_message>
<xml_diff>
--- a/Naukri Login.xlsx
+++ b/Naukri Login.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="6">
   <si>
     <t>Username</t>
   </si>
@@ -371,7 +371,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C232"/>
+  <dimension ref="A1:C258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -2239,6 +2239,214 @@
         <v>5</v>
       </c>
     </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>4</v>
+      </c>
+      <c r="B233" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>4</v>
+      </c>
+      <c r="B234" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s">
+        <v>4</v>
+      </c>
+      <c r="B235" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s">
+        <v>4</v>
+      </c>
+      <c r="B236" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>4</v>
+      </c>
+      <c r="B237" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>4</v>
+      </c>
+      <c r="B238" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>4</v>
+      </c>
+      <c r="B239" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s">
+        <v>4</v>
+      </c>
+      <c r="B240" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s">
+        <v>4</v>
+      </c>
+      <c r="B241" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="s">
+        <v>4</v>
+      </c>
+      <c r="B242" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="s">
+        <v>4</v>
+      </c>
+      <c r="B243" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s">
+        <v>4</v>
+      </c>
+      <c r="B244" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s">
+        <v>4</v>
+      </c>
+      <c r="B245" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="s">
+        <v>4</v>
+      </c>
+      <c r="B246" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="s">
+        <v>4</v>
+      </c>
+      <c r="B247" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="s">
+        <v>4</v>
+      </c>
+      <c r="B248" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s">
+        <v>4</v>
+      </c>
+      <c r="B249" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="s">
+        <v>4</v>
+      </c>
+      <c r="B250" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="s">
+        <v>4</v>
+      </c>
+      <c r="B251" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s">
+        <v>4</v>
+      </c>
+      <c r="B252" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="s">
+        <v>4</v>
+      </c>
+      <c r="B253" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="s">
+        <v>4</v>
+      </c>
+      <c r="B254" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s">
+        <v>4</v>
+      </c>
+      <c r="B255" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s">
+        <v>4</v>
+      </c>
+      <c r="B256" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s">
+        <v>4</v>
+      </c>
+      <c r="B257" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s">
+        <v>4</v>
+      </c>
+      <c r="B258" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A2"/>

</xml_diff>